<commit_message>
Cập nhật danh sách IP
</commit_message>
<xml_diff>
--- a/DOCS-OPS-Mitaka/tools/IP-Planning.xlsx
+++ b/DOCS-OPS-Mitaka/tools/IP-Planning.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IP-Planning" sheetId="1" r:id="rId1"/>
+    <sheet name="Draft" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
   <si>
     <t>Controller</t>
   </si>
@@ -90,13 +91,16 @@
   </si>
   <si>
     <t>Compute1</t>
+  </si>
+  <si>
+    <t>HDD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +121,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +142,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -327,11 +344,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -340,9 +394,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -350,6 +401,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -359,35 +443,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -705,197 +777,197 @@
       </c>
     </row>
     <row r="6" spans="3:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="9"/>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="15" t="s">
+      <c r="E7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="10"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
-      <c r="D10" s="19" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="E10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -905,4 +977,249 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="3:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C14:H14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cấu hình phần cứng
</commit_message>
<xml_diff>
--- a/DOCS-OPS-Mitaka/tools/IP-Planning.xlsx
+++ b/DOCS-OPS-Mitaka/tools/IP-Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="IP-Planning" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
   <si>
     <t>Controller</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>HDD</t>
+  </si>
+  <si>
+    <t>Swift2</t>
   </si>
 </sst>
 </file>
@@ -443,6 +446,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -451,15 +463,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +776,7 @@
         <v>9</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="3:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -983,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,18 +1015,18 @@
         <v>9</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="3:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="14" t="s">
@@ -1086,14 +1089,14 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="14" t="s">
@@ -1156,14 +1159,14 @@
       </c>
     </row>
     <row r="14" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5"/>

</xml_diff>

<commit_message>
Cập nhật chú ý
</commit_message>
<xml_diff>
--- a/DOCS-OPS-Mitaka/tools/IP-Planning.xlsx
+++ b/DOCS-OPS-Mitaka/tools/IP-Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="36">
   <si>
     <t>Controller</t>
   </si>
@@ -97,13 +97,49 @@
   </si>
   <si>
     <t>Swift2</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>+100GB</t>
+  </si>
+  <si>
+    <t>+2GB</t>
+  </si>
+  <si>
+    <t>+4GB</t>
+  </si>
+  <si>
+    <t>+50GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dev/sdb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dev/sda </t>
+  </si>
+  <si>
+    <t>/dev/sdc</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>+2CPU</t>
+  </si>
+  <si>
+    <t>+4CPU</t>
+  </si>
+  <si>
+    <t>CẤU HÌNH PHẦN CỨNG - OPENSTACK MITAKA LAB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +167,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +194,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -384,11 +433,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,9 +495,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,6 +528,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -463,6 +557,57 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:I18"/>
+  <dimension ref="C4:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +905,17 @@
     <col min="9" max="9" width="23" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="3:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
+    </row>
     <row r="5" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -783,64 +939,64 @@
       <c r="C6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="33" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="19"/>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="11" t="s">
+      <c r="E7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="35" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="20"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="37" t="s">
         <v>2</v>
       </c>
     </row>
@@ -848,134 +1004,207 @@
       <c r="C9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="17"/>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="11" t="s">
+      <c r="E10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="35" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="17"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="C13" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="C14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="40" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1029,62 +1258,62 @@
       <c r="H6" s="23"/>
     </row>
     <row r="7" spans="3:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1099,62 +1328,62 @@
       <c r="H10" s="23"/>
     </row>
     <row r="11" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="11" t="s">
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1178,43 +1407,43 @@
     </row>
     <row r="16" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>